<commit_message>
Modificación documento de excel
Se modifica hoja cursos del archivo
Documentacion.xls
</commit_message>
<xml_diff>
--- a/documentos/documentacion.xlsx
+++ b/documentos/documentacion.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planteamiento del proyecto" sheetId="1" r:id="rId1"/>
     <sheet name="Esquema de actividades" sheetId="2" r:id="rId2"/>
     <sheet name="cursos" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
   <si>
     <t>PROYECTO INTRAWEB</t>
   </si>
@@ -545,6 +545,21 @@
   </si>
   <si>
     <t>23/05/2016</t>
+  </si>
+  <si>
+    <t>DRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>SOLID</t>
+  </si>
+  <si>
+    <t>Tecnicas de user experience</t>
+  </si>
+  <si>
+    <t>Diseño de interaccion</t>
   </si>
 </sst>
 </file>
@@ -759,6 +774,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,22 +801,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E2F3"/>
+          <bgColor rgb="FFD9E2F3"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -841,17 +903,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A4:H42" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A4:H42" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A4:H42"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="fase" dataDxfId="5"/>
-    <tableColumn id="2" name="Actividad" dataDxfId="6"/>
-    <tableColumn id="3" name="fecha de inicio" dataDxfId="4"/>
-    <tableColumn id="4" name="fecha de finalizado" dataDxfId="9"/>
-    <tableColumn id="5" name="Estimacion" dataDxfId="3"/>
-    <tableColumn id="6" name="comentarios" dataDxfId="2"/>
-    <tableColumn id="7" name="log de defectos" dataDxfId="1"/>
-    <tableColumn id="8" name="estado y descripcion de solucion" dataDxfId="0"/>
+    <tableColumn id="1" name="fase" dataDxfId="9"/>
+    <tableColumn id="2" name="Actividad" dataDxfId="8"/>
+    <tableColumn id="3" name="fecha de inicio" dataDxfId="7"/>
+    <tableColumn id="4" name="fecha de finalizado" dataDxfId="6"/>
+    <tableColumn id="5" name="Estimacion" dataDxfId="5"/>
+    <tableColumn id="6" name="comentarios" dataDxfId="4"/>
+    <tableColumn id="7" name="log de defectos" dataDxfId="3"/>
+    <tableColumn id="8" name="estado y descripcion de solucion" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B3:G18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:G18"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Cursos" dataDxfId="1"/>
+    <tableColumn id="2" name="Cursos2"/>
+    <tableColumn id="3" name="fecha inicio"/>
+    <tableColumn id="4" name="fecha fin"/>
+    <tableColumn id="5" name="sitios"/>
+    <tableColumn id="6" name="comentarios"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1122,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1153,24 +1230,24 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="24"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -1181,57 +1258,57 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="20"/>
       <c r="G5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="20"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="20"/>
       <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="15"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="16"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1240,11 +1317,11 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1253,40 +1330,40 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="20"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="16"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="15"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1296,14 +1373,14 @@
       <c r="G14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="21"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="26" t="s">
         <v>163</v>
       </c>
       <c r="G15" s="2">
@@ -1314,11 +1391,11 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="2">
         <v>25</v>
       </c>
@@ -1327,11 +1404,11 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="2">
         <v>23</v>
       </c>
@@ -1340,11 +1417,11 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="2">
         <v>17</v>
       </c>
@@ -1353,11 +1430,11 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="2">
         <v>14</v>
       </c>
@@ -1366,11 +1443,11 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="15"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="2">
         <v>10</v>
       </c>
@@ -1379,11 +1456,11 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="2">
         <v>5</v>
       </c>
@@ -1392,11 +1469,11 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="16"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="2">
         <v>3</v>
       </c>
@@ -1405,7 +1482,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1414,8 +1491,8 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="25" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F24" s="1"/>
@@ -1423,10 +1500,10 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F25" s="1"/>
@@ -7301,8 +7378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7351,123 +7428,123 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="15" t="s">
         <v>168</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="J5" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="15" t="s">
         <v>168</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
       <c r="J6" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="15" t="s">
         <v>168</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
       <c r="J7" s="11" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="15" t="s">
         <v>168</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
       <c r="J8" s="11" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="15" t="s">
         <v>168</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C10" s="11"/>
@@ -7475,16 +7552,16 @@
       <c r="E10" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
       <c r="J10" s="11" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="14" t="s">
         <v>155</v>
       </c>
       <c r="C11" s="11" t="s">
@@ -7492,20 +7569,20 @@
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="16" t="s">
         <v>166</v>
       </c>
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="14" t="s">
         <v>64</v>
       </c>
       <c r="C12" s="11"/>
@@ -7513,13 +7590,13 @@
       <c r="E12" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="14" t="s">
         <v>161</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -7529,17 +7606,17 @@
       <c r="E13" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="14" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="11"/>
@@ -7547,13 +7624,13 @@
       <c r="E14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C15" s="11"/>
@@ -7561,13 +7638,13 @@
       <c r="E15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C16" s="11"/>
@@ -7575,13 +7652,13 @@
       <c r="E16" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="11"/>
@@ -7589,15 +7666,15 @@
       <c r="E17" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="14" t="s">
         <v>74</v>
       </c>
       <c r="C18" s="11"/>
@@ -7605,15 +7682,15 @@
       <c r="E18" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="11"/>
@@ -7621,13 +7698,13 @@
       <c r="E19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C20" s="11"/>
@@ -7635,17 +7712,17 @@
       <c r="E20" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="14" t="s">
         <v>80</v>
       </c>
       <c r="C21" s="11"/>
@@ -7653,13 +7730,13 @@
       <c r="E21" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C22" s="11"/>
@@ -7667,15 +7744,15 @@
       <c r="E22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C23" s="11"/>
@@ -7683,15 +7760,15 @@
       <c r="E23" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="11"/>
@@ -7699,13 +7776,13 @@
       <c r="E24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="11"/>
@@ -7713,17 +7790,17 @@
       <c r="E25" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
     </row>
     <row r="26" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="14" t="s">
         <v>90</v>
       </c>
       <c r="C26" s="11"/>
@@ -7731,15 +7808,15 @@
       <c r="E26" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="14" t="s">
         <v>92</v>
       </c>
       <c r="C27" s="11"/>
@@ -7747,15 +7824,15 @@
       <c r="E27" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="14" t="s">
         <v>94</v>
       </c>
       <c r="C28" s="11"/>
@@ -7763,15 +7840,15 @@
       <c r="E28" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C29" s="11"/>
@@ -7779,15 +7856,15 @@
       <c r="E29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="14" t="s">
         <v>97</v>
       </c>
       <c r="C30" s="11"/>
@@ -7795,15 +7872,15 @@
       <c r="E30" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
     </row>
     <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="14" t="s">
         <v>100</v>
       </c>
       <c r="C31" s="11"/>
@@ -7811,15 +7888,15 @@
       <c r="E31" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="14" t="s">
         <v>103</v>
       </c>
       <c r="C32" s="11"/>
@@ -7827,15 +7904,15 @@
       <c r="E32" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
     </row>
     <row r="33" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="14" t="s">
         <v>106</v>
       </c>
       <c r="C33" s="11"/>
@@ -7843,15 +7920,15 @@
       <c r="E33" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="14" t="s">
         <v>109</v>
       </c>
       <c r="C34" s="11"/>
@@ -7859,17 +7936,17 @@
       <c r="E34" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
     </row>
     <row r="35" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="14" t="s">
         <v>112</v>
       </c>
       <c r="C35" s="11"/>
@@ -7877,15 +7954,15 @@
       <c r="E35" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
     </row>
     <row r="36" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="14" t="s">
         <v>114</v>
       </c>
       <c r="C36" s="11"/>
@@ -7893,15 +7970,15 @@
       <c r="E36" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="14" t="s">
         <v>115</v>
       </c>
       <c r="C37" s="11"/>
@@ -7909,17 +7986,17 @@
       <c r="E37" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="14" t="s">
         <v>117</v>
       </c>
       <c r="C38" s="11"/>
@@ -7927,13 +8004,13 @@
       <c r="E38" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="14" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="11"/>
@@ -7941,13 +8018,13 @@
       <c r="E39" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C40" s="11"/>
@@ -7955,13 +8032,13 @@
       <c r="E40" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="14" t="s">
         <v>120</v>
       </c>
       <c r="C41" s="11"/>
@@ -7969,15 +8046,15 @@
       <c r="E41" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="14" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="11"/>
@@ -7985,9 +8062,9 @@
       <c r="E42" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8001,17 +8078,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
     <col min="7" max="7" width="65.42578125" customWidth="1"/>
     <col min="8" max="26" width="9.42578125" customWidth="1"/>
@@ -8224,24 +8301,34 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>170</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
+      <c r="B17" s="7" t="s">
+        <v>171</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+    <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>173</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -16105,5 +16192,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>